<commit_message>
Inserção do SqlLite para guardar os dados historicos
</commit_message>
<xml_diff>
--- a/templates/template.xlsx
+++ b/templates/template.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Meu Drive\06. PROJETOS\Condominio\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Meu Drive\06. PROJETOS\Condominio\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C16187D0-A5C9-4AC2-8491-78B9E797877E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25959ABC-1DDB-4F65-8C92-77EBF6A0027A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -85,9 +85,6 @@
     <t>Mes Ano Atual</t>
   </si>
   <si>
-    <t>01-2026</t>
-  </si>
-  <si>
     <t>Valor do Mes anterior</t>
   </si>
   <si>
@@ -182,13 +179,16 @@
   </si>
   <si>
     <t>Ano Atrasado</t>
+  </si>
+  <si>
+    <t>02-2026</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -219,6 +219,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -266,7 +272,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -275,10 +281,6 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
@@ -300,6 +302,9 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -520,7 +525,7 @@
   <dimension ref="A1:M1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13:C24"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -562,354 +567,354 @@
         <v>6</v>
       </c>
       <c r="K1" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="L1" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="M1" s="6" t="s">
         <v>39</v>
-      </c>
-      <c r="M1" s="6" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="E2" s="11">
+      <c r="B2" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2" s="9">
         <v>1680</v>
       </c>
-      <c r="G2" s="13"/>
-      <c r="H2" s="13"/>
-      <c r="I2" s="13"/>
-      <c r="K2" s="12">
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="K2" s="10">
         <v>15</v>
       </c>
-      <c r="L2" s="10">
+      <c r="L2" s="8">
         <v>1</v>
       </c>
-      <c r="M2" s="12">
+      <c r="M2" s="10">
         <v>2025</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="10">
+        <v>8</v>
+      </c>
+      <c r="B3" s="8">
         <v>11500.5</v>
       </c>
-      <c r="D3" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="E3" s="11">
+      <c r="D3" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="E3" s="9">
         <v>111.53</v>
       </c>
-      <c r="G3" s="14">
+      <c r="G3" s="12">
         <v>8</v>
       </c>
-      <c r="H3" s="15">
+      <c r="H3" s="13">
         <v>1</v>
       </c>
-      <c r="I3" s="14">
+      <c r="I3" s="12">
         <v>2025</v>
       </c>
-      <c r="K3" s="12">
+      <c r="K3" s="10">
         <v>16</v>
       </c>
-      <c r="L3" s="12">
+      <c r="L3" s="10">
         <v>2</v>
       </c>
-      <c r="M3" s="12">
+      <c r="M3" s="10">
         <v>2024</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="D4" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" s="11">
+      <c r="D4" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="9">
         <v>99.99</v>
       </c>
-      <c r="G4" s="14">
+      <c r="G4" s="12">
         <v>8</v>
       </c>
-      <c r="H4" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="I4" s="14">
+      <c r="H4" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="I4" s="12">
         <v>2025</v>
       </c>
-      <c r="K4" s="12">
+      <c r="K4" s="10">
         <v>16</v>
       </c>
-      <c r="L4" s="12">
+      <c r="L4" s="10">
         <v>3</v>
       </c>
-      <c r="M4" s="12">
+      <c r="M4" s="10">
         <v>2024</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="3"/>
+      <c r="D5" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="9">
+        <v>240</v>
+      </c>
+      <c r="G5" s="12">
+        <v>8</v>
+      </c>
+      <c r="H5" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="3"/>
-      <c r="D5" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="E5" s="11">
-        <v>240</v>
-      </c>
-      <c r="G5" s="14">
-        <v>8</v>
-      </c>
-      <c r="H5" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="I5" s="14">
+      <c r="I5" s="12">
         <v>2025</v>
       </c>
-      <c r="K5" s="12">
+      <c r="K5" s="10">
         <v>16</v>
       </c>
-      <c r="L5" s="12">
+      <c r="L5" s="10">
         <v>4</v>
       </c>
-      <c r="M5" s="12">
+      <c r="M5" s="10">
         <v>2025</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B6" s="7">
         <v>28</v>
       </c>
-      <c r="D6" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="E6" s="11">
+      <c r="D6" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6" s="9">
         <v>399.4</v>
       </c>
-      <c r="G6" s="14">
+      <c r="G6" s="12">
         <v>8</v>
       </c>
-      <c r="H6" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="I6" s="14">
+      <c r="H6" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="I6" s="12">
         <v>2025</v>
       </c>
-      <c r="K6" s="12"/>
-      <c r="L6" s="12"/>
-      <c r="M6" s="12"/>
+      <c r="K6" s="10"/>
+      <c r="L6" s="10"/>
+      <c r="M6" s="10"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" s="8" cm="1">
+        <v>16</v>
+      </c>
+      <c r="B7" s="3" cm="1">
         <f t="array" ref="B7">SUMPRODUCT((K2:K15&lt;&gt;"")*(L2:L15&lt;&gt;"")*(M2:M15&lt;&gt;""))</f>
         <v>4</v>
       </c>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
-      <c r="G7" s="14">
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="G7" s="12">
         <v>8</v>
       </c>
-      <c r="H7" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="I7" s="14">
+      <c r="H7" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="I7" s="12">
         <v>2025</v>
       </c>
-      <c r="K7" s="12"/>
-      <c r="L7" s="12"/>
-      <c r="M7" s="12"/>
+      <c r="K7" s="10"/>
+      <c r="L7" s="10"/>
+      <c r="M7" s="10"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="7">
+        <v>3</v>
+      </c>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="G8" s="12">
+        <v>8</v>
+      </c>
+      <c r="H8" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="7">
-        <v>0</v>
-      </c>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
-      <c r="G8" s="14">
+      <c r="I8" s="12">
+        <v>2026</v>
+      </c>
+      <c r="K8" s="10"/>
+      <c r="L8" s="14"/>
+      <c r="M8" s="10"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="G9" s="12">
         <v>8</v>
       </c>
-      <c r="H8" s="15" t="s">
+      <c r="H9" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="I8" s="14">
+      <c r="I9" s="12">
         <v>2026</v>
       </c>
-      <c r="K8" s="12"/>
-      <c r="L8" s="16"/>
-      <c r="M8" s="12"/>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="G9" s="14">
-        <v>8</v>
-      </c>
-      <c r="H9" s="15" t="s">
+      <c r="K9" s="10"/>
+      <c r="L9" s="10"/>
+      <c r="M9" s="10"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="G10" s="12">
+        <v>18</v>
+      </c>
+      <c r="H10" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="I9" s="14">
+      <c r="I10" s="12">
+        <v>2025</v>
+      </c>
+      <c r="K10" s="10"/>
+      <c r="L10" s="10"/>
+      <c r="M10" s="10"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="D11" s="10"/>
+      <c r="E11" s="10"/>
+      <c r="G11" s="12">
+        <v>18</v>
+      </c>
+      <c r="H11" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="I11" s="12">
+        <v>2025</v>
+      </c>
+      <c r="K11" s="10"/>
+      <c r="L11" s="10"/>
+      <c r="M11" s="10"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="D12" s="10"/>
+      <c r="E12" s="10"/>
+      <c r="G12" s="12">
+        <v>18</v>
+      </c>
+      <c r="H12" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="I12" s="12">
         <v>2026</v>
       </c>
-      <c r="K9" s="12"/>
-      <c r="L9" s="12"/>
-      <c r="M9" s="12"/>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="G10" s="14">
-        <v>18</v>
-      </c>
-      <c r="H10" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="I10" s="14">
-        <v>2025</v>
-      </c>
-      <c r="K10" s="12"/>
-      <c r="L10" s="12"/>
-      <c r="M10" s="12"/>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="D11" s="12"/>
-      <c r="E11" s="12"/>
-      <c r="G11" s="14">
-        <v>18</v>
-      </c>
-      <c r="H11" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="I11" s="14">
-        <v>2025</v>
-      </c>
-      <c r="K11" s="12"/>
-      <c r="L11" s="12"/>
-      <c r="M11" s="12"/>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="D12" s="12"/>
-      <c r="E12" s="12"/>
-      <c r="G12" s="14">
-        <v>18</v>
-      </c>
-      <c r="H12" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="I12" s="14">
-        <v>2026</v>
-      </c>
-      <c r="K12" s="12"/>
-      <c r="L12" s="12"/>
-      <c r="M12" s="12"/>
+      <c r="K12" s="10"/>
+      <c r="L12" s="10"/>
+      <c r="M12" s="10"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="D13" s="12"/>
-      <c r="E13" s="12"/>
-      <c r="G13" s="12"/>
-      <c r="H13" s="12"/>
-      <c r="I13" s="12"/>
-      <c r="K13" s="12"/>
-      <c r="L13" s="12"/>
-      <c r="M13" s="12"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="10"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="10"/>
+      <c r="I13" s="10"/>
+      <c r="K13" s="10"/>
+      <c r="L13" s="10"/>
+      <c r="M13" s="10"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="D14" s="12"/>
-      <c r="E14" s="12"/>
-      <c r="G14" s="12"/>
-      <c r="H14" s="12"/>
-      <c r="I14" s="12"/>
-      <c r="K14" s="12"/>
-      <c r="L14" s="12"/>
-      <c r="M14" s="12"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="10"/>
+      <c r="G14" s="10"/>
+      <c r="H14" s="10"/>
+      <c r="I14" s="10"/>
+      <c r="K14" s="10"/>
+      <c r="L14" s="10"/>
+      <c r="M14" s="10"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="D15" s="12"/>
-      <c r="E15" s="12"/>
-      <c r="G15" s="12"/>
-      <c r="H15" s="12"/>
-      <c r="I15" s="12"/>
-      <c r="K15" s="12"/>
-      <c r="L15" s="12"/>
-      <c r="M15" s="12"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="10"/>
+      <c r="I15" s="10"/>
+      <c r="K15" s="10"/>
+      <c r="L15" s="10"/>
+      <c r="M15" s="10"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="D16" s="12"/>
-      <c r="E16" s="12"/>
-      <c r="G16" s="12"/>
-      <c r="H16" s="12"/>
-      <c r="I16" s="12"/>
-      <c r="K16" s="12"/>
-      <c r="L16" s="12"/>
-      <c r="M16" s="12"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="10"/>
+      <c r="G16" s="10"/>
+      <c r="H16" s="10"/>
+      <c r="I16" s="10"/>
+      <c r="K16" s="10"/>
+      <c r="L16" s="10"/>
+      <c r="M16" s="10"/>
     </row>
     <row r="17" spans="4:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D17" s="12"/>
-      <c r="E17" s="12"/>
-      <c r="G17" s="12"/>
-      <c r="H17" s="12"/>
-      <c r="I17" s="12"/>
-      <c r="K17" s="12"/>
-      <c r="L17" s="12"/>
-      <c r="M17" s="12"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="10"/>
+      <c r="G17" s="10"/>
+      <c r="H17" s="10"/>
+      <c r="I17" s="10"/>
+      <c r="K17" s="10"/>
+      <c r="L17" s="10"/>
+      <c r="M17" s="10"/>
     </row>
     <row r="18" spans="4:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D18" s="12"/>
-      <c r="E18" s="12"/>
-      <c r="G18" s="12"/>
-      <c r="H18" s="12"/>
-      <c r="I18" s="12"/>
-      <c r="K18" s="12"/>
-      <c r="L18" s="12"/>
-      <c r="M18" s="12"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="10"/>
+      <c r="G18" s="10"/>
+      <c r="H18" s="10"/>
+      <c r="I18" s="10"/>
+      <c r="K18" s="10"/>
+      <c r="L18" s="10"/>
+      <c r="M18" s="10"/>
     </row>
     <row r="19" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="D19" s="12"/>
-      <c r="E19" s="12"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="10"/>
       <c r="F19" s="4"/>
-      <c r="G19" s="12"/>
-      <c r="H19" s="12"/>
-      <c r="I19" s="12"/>
-      <c r="K19" s="12"/>
-      <c r="L19" s="12"/>
-      <c r="M19" s="12"/>
+      <c r="G19" s="10"/>
+      <c r="H19" s="10"/>
+      <c r="I19" s="10"/>
+      <c r="K19" s="10"/>
+      <c r="L19" s="10"/>
+      <c r="M19" s="10"/>
     </row>
     <row r="20" spans="4:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D20" s="12"/>
-      <c r="E20" s="12"/>
-      <c r="G20" s="12"/>
-      <c r="H20" s="12"/>
-      <c r="I20" s="12"/>
-      <c r="K20" s="12"/>
-      <c r="L20" s="12"/>
-      <c r="M20" s="12"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="10"/>
+      <c r="G20" s="10"/>
+      <c r="H20" s="10"/>
+      <c r="I20" s="10"/>
+      <c r="K20" s="10"/>
+      <c r="L20" s="10"/>
+      <c r="M20" s="10"/>
     </row>
     <row r="21" spans="4:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D21" s="12"/>
-      <c r="E21" s="12"/>
-      <c r="G21" s="12"/>
-      <c r="H21" s="12"/>
-      <c r="I21" s="12"/>
-      <c r="K21" s="12"/>
-      <c r="L21" s="12"/>
-      <c r="M21" s="12"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="10"/>
+      <c r="G21" s="10"/>
+      <c r="H21" s="10"/>
+      <c r="I21" s="10"/>
+      <c r="K21" s="10"/>
+      <c r="L21" s="10"/>
+      <c r="M21" s="10"/>
     </row>
     <row r="22" spans="4:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="23" spans="4:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1923,12 +1928,12 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B2" s="1">
         <v>100</v>
@@ -1936,7 +1941,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B3" s="1">
         <v>122</v>
@@ -1944,7 +1949,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B4" s="1">
         <v>20</v>
@@ -1952,34 +1957,34 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>